<commit_message>
removed age calculation, all works
</commit_message>
<xml_diff>
--- a/Result/Hearing_data.xlsx
+++ b/Result/Hearing_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14120"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Median_Male" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Hz</t>
   </si>
@@ -61,16 +61,82 @@
     <t>𝛾_5</t>
   </si>
   <si>
-    <t>α</t>
-  </si>
-  <si>
-    <t>β</t>
-  </si>
-  <si>
     <t>alpha</t>
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>0.000398</t>
+  </si>
+  <si>
+    <t>0.000261</t>
+  </si>
+  <si>
+    <t>0.000221</t>
+  </si>
+  <si>
+    <t>0.000312</t>
+  </si>
+  <si>
+    <t>0.00253</t>
+  </si>
+  <si>
+    <t>0.000737</t>
+  </si>
+  <si>
+    <t>0.000139</t>
+  </si>
+  <si>
+    <t>0.000459</t>
+  </si>
+  <si>
+    <t>0.000702</t>
+  </si>
+  <si>
+    <t>0.00156</t>
+  </si>
+  <si>
+    <t>0.00506</t>
+  </si>
+  <si>
+    <t>0.0034</t>
+  </si>
+  <si>
+    <t>2.832</t>
+  </si>
+  <si>
+    <t>2.537</t>
+  </si>
+  <si>
+    <t>2.494</t>
+  </si>
+  <si>
+    <t>2.404</t>
+  </si>
+  <si>
+    <t>2.325</t>
+  </si>
+  <si>
+    <t>2.328</t>
+  </si>
+  <si>
+    <t>2.568</t>
+  </si>
+  <si>
+    <t>2.708</t>
+  </si>
+  <si>
+    <t>2.805</t>
+  </si>
+  <si>
+    <t>2.792</t>
+  </si>
+  <si>
+    <t>2.66</t>
+  </si>
+  <si>
+    <t>2.439</t>
   </si>
 </sst>
 </file>
@@ -139,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -150,6 +216,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,123 +531,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>250</v>
       </c>
-      <c r="B2" s="2">
-        <f>1.39*10^-4</f>
-        <v>1.3899999999999999E-4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2.8319999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>500</v>
       </c>
-      <c r="B3" s="2">
-        <f>4.59*10^-4</f>
-        <v>4.5899999999999999E-4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2.5369999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1000</v>
       </c>
-      <c r="B4" s="2">
-        <f>7.02*10^-4</f>
-        <v>7.0200000000000004E-4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2.4940000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
-      <c r="B5" s="2">
-        <f>1.56*10^-3</f>
-        <v>1.5600000000000002E-3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2.4039999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4000</v>
       </c>
-      <c r="B6" s="2">
-        <f>3.4*10^-3</f>
-        <v>3.3999999999999998E-3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2.3250000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>8000</v>
       </c>
-      <c r="B7" s="2">
-        <f>5.06*10^-3</f>
-        <v>5.0599999999999994E-3</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2.3279999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -597,15 +664,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,77 +683,77 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>250</v>
       </c>
-      <c r="B2" s="2">
-        <f>3.98*10^-4</f>
-        <v>3.9800000000000002E-4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2.5680000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>500</v>
       </c>
-      <c r="B3" s="2">
-        <f>2.61*10^-4</f>
-        <v>2.61E-4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2.7080000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1000</v>
       </c>
-      <c r="B4" s="2">
-        <f>2.21*10^-4</f>
-        <v>2.2100000000000001E-4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2.8050000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
-      <c r="B5" s="2">
-        <f>3.12*10^-4</f>
-        <v>3.1200000000000005E-4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2.7919999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4000</v>
       </c>
-      <c r="B6" s="2">
-        <f>7.37*10^-4</f>
-        <v>7.3700000000000002E-4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2.66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>8000</v>
       </c>
-      <c r="B7" s="2">
-        <f>2.53*10^-3</f>
-        <v>2.5299999999999997E-3</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2.4390000000000001</v>
-      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>